<commit_message>
Updated MassTransit tests with results for non-durable (transient) messaging.
</commit_message>
<xml_diff>
--- a/data/RabbitMQ/Payload benchmarks data.xlsx
+++ b/data/RabbitMQ/Payload benchmarks data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Payload_Raw_Data" sheetId="1" r:id="rId1"/>
@@ -954,19 +954,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.34</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.83</c:v>
+                  <c:v>26.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.64</c:v>
+                  <c:v>172.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136.26</c:v>
+                  <c:v>301.23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>153.88999999999999</c:v>
+                  <c:v>224.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1131,11 +1131,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="149296240"/>
-        <c:axId val="324781264"/>
+        <c:axId val="211144160"/>
+        <c:axId val="211144720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="149296240"/>
+        <c:axId val="211144160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1239,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324781264"/>
+        <c:crossAx val="211144720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1247,7 +1247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324781264"/>
+        <c:axId val="211144720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1354,7 +1354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149296240"/>
+        <c:crossAx val="211144160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2281,7 +2281,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,38 +2521,38 @@
         <v>2</v>
       </c>
       <c r="B8" s="4">
-        <v>28.348299999999998</v>
+        <v>13.8127</v>
       </c>
       <c r="C8" s="4">
-        <v>28.5504</v>
+        <v>13.8803</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3">
-        <v>28.258199999999999</v>
+        <v>14.6549</v>
       </c>
       <c r="F8" s="3">
-        <v>28.244</v>
+        <v>14.5397</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="4">
-        <v>55.503999999999998</v>
+        <v>22.162199999999999</v>
       </c>
       <c r="I8" s="4">
-        <v>55.649500000000003</v>
+        <v>22.087700000000002</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3">
-        <v>279.93200000000002</v>
+        <v>126.7817</v>
       </c>
       <c r="L8" s="3">
-        <v>279.9812</v>
+        <v>126.4907</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="4">
-        <v>2570.1491999999998</v>
+        <v>1835.8768</v>
       </c>
       <c r="O8" s="4">
-        <v>2628.4418999999998</v>
+        <v>1730.587</v>
       </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -2711,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,63 +3044,63 @@
       </c>
       <c r="B8">
         <f>AVERAGE(Payload_Raw_Data!B8:C8)</f>
-        <v>28.449349999999999</v>
+        <v>13.846499999999999</v>
       </c>
       <c r="C8">
         <f>AVERAGE(Payload_Raw_Data!E8:F8)</f>
-        <v>28.251100000000001</v>
+        <v>14.597300000000001</v>
       </c>
       <c r="D8">
         <f>AVERAGE(Payload_Raw_Data!H8:I8)</f>
-        <v>55.576750000000004</v>
+        <v>22.124949999999998</v>
       </c>
       <c r="E8">
         <f>AVERAGE(Payload_Raw_Data!K8:L8)</f>
-        <v>279.95659999999998</v>
+        <v>126.6362</v>
       </c>
       <c r="F8">
         <f>AVERAGE(Payload_Raw_Data!N8:O8)</f>
-        <v>2599.2955499999998</v>
+        <v>1783.2319</v>
       </c>
       <c r="H8">
         <f t="shared" si="8"/>
-        <v>7030.04</v>
+        <v>14444.08</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>7079.37</v>
+        <v>13701.16</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>3598.63</v>
+        <v>9039.57</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>714.4</v>
+        <v>1579.33</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>76.94</v>
+        <v>112.16</v>
       </c>
       <c r="N8">
         <f t="shared" si="9"/>
-        <v>1.34</v>
+        <v>2.75</v>
       </c>
       <c r="O8">
         <f t="shared" si="4"/>
-        <v>13.83</v>
+        <v>26.76</v>
       </c>
       <c r="P8">
         <f t="shared" si="5"/>
-        <v>68.64</v>
+        <v>172.42</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>136.26</v>
+        <v>301.23</v>
       </c>
       <c r="R8">
         <f t="shared" si="7"/>
-        <v>153.88999999999999</v>
+        <v>224.31</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3177,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,23 +3322,23 @@
       </c>
       <c r="B8">
         <f>Payload_Plot_Source!N8</f>
-        <v>1.34</v>
+        <v>2.75</v>
       </c>
       <c r="C8">
         <f>Payload_Plot_Source!O8</f>
-        <v>13.83</v>
+        <v>26.76</v>
       </c>
       <c r="D8">
         <f>Payload_Plot_Source!P8</f>
-        <v>68.64</v>
+        <v>172.42</v>
       </c>
       <c r="E8">
         <f>Payload_Plot_Source!Q8</f>
-        <v>136.26</v>
+        <v>301.23</v>
       </c>
       <c r="F8">
         <f>Payload_Plot_Source!R8</f>
-        <v>153.88999999999999</v>
+        <v>224.31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>